<commit_message>
fixed error in raw ADC channel map
</commit_message>
<xml_diff>
--- a/doc/chamber_channel_map.xlsx
+++ b/doc/chamber_channel_map.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madorsky/github/wib_sim/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\wib_felix\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B4D451-C154-D844-8A8E-DB7B69C20148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-12820" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-12825" windowWidth="38400" windowHeight="21600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Modular FEMB" sheetId="5" r:id="rId1"/>
     <sheet name="Monolithic FEMB" sheetId="6" r:id="rId2"/>
     <sheet name="raw channel" sheetId="7" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -95,7 +94,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
@@ -159,11 +158,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Heading1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Heading" xfId="1"/>
+    <cellStyle name="Heading1" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Result" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Result2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Result" xfId="3"/>
+    <cellStyle name="Result2" xfId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -474,23 +473,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K129"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="8.83203125" style="1"/>
-    <col min="6" max="8" width="8.83203125" style="1"/>
-    <col min="9" max="9" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="54.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="8.875" style="1"/>
+    <col min="6" max="8" width="8.875" style="1"/>
+    <col min="9" max="9" width="14.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="54.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,7 +524,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -566,7 +565,7 @@
         <v>// U0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -607,7 +606,7 @@
         <v>// U1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -648,7 +647,7 @@
         <v>// U2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -689,7 +688,7 @@
         <v>// U3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -730,7 +729,7 @@
         <v>// U4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -771,7 +770,7 @@
         <v>// U5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -812,7 +811,7 @@
         <v>// U6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -853,7 +852,7 @@
         <v>// U7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -894,7 +893,7 @@
         <v>// U8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -935,7 +934,7 @@
         <v>// U9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -976,7 +975,7 @@
         <v>// U10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -1017,7 +1016,7 @@
         <v>// U11</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -1058,7 +1057,7 @@
         <v>// U12</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>// U13</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -1140,7 +1139,7 @@
         <v>// U14</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -1181,7 +1180,7 @@
         <v>// U15</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1222,7 +1221,7 @@
         <v>// U16</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>// U17</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1304,7 +1303,7 @@
         <v>// U18</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2</v>
       </c>
@@ -1345,7 +1344,7 @@
         <v>// U19</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>4</v>
       </c>
@@ -1386,7 +1385,7 @@
         <v>// U20</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>6</v>
       </c>
@@ -1427,7 +1426,7 @@
         <v>// U21</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>4</v>
       </c>
@@ -1468,7 +1467,7 @@
         <v>// U22</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>6</v>
       </c>
@@ -1509,7 +1508,7 @@
         <v>// U23</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>4</v>
       </c>
@@ -1550,7 +1549,7 @@
         <v>// U24</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>6</v>
       </c>
@@ -1591,7 +1590,7 @@
         <v>// U25</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>4</v>
       </c>
@@ -1632,7 +1631,7 @@
         <v>// U26</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>6</v>
       </c>
@@ -1673,7 +1672,7 @@
         <v>// U27</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>4</v>
       </c>
@@ -1714,7 +1713,7 @@
         <v>// U28</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>6</v>
       </c>
@@ -1755,7 +1754,7 @@
         <v>// U29</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>5</v>
       </c>
@@ -1796,7 +1795,7 @@
         <v>// U30</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>7</v>
       </c>
@@ -1837,7 +1836,7 @@
         <v>// U31</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>5</v>
       </c>
@@ -1878,7 +1877,7 @@
         <v>// U32</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>7</v>
       </c>
@@ -1919,7 +1918,7 @@
         <v>// U33</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>5</v>
       </c>
@@ -1960,7 +1959,7 @@
         <v>// U34</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>7</v>
       </c>
@@ -2001,7 +2000,7 @@
         <v>// U35</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>5</v>
       </c>
@@ -2042,7 +2041,7 @@
         <v>// U36</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>7</v>
       </c>
@@ -2083,7 +2082,7 @@
         <v>// U37</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>5</v>
       </c>
@@ -2124,7 +2123,7 @@
         <v>// U38</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>7</v>
       </c>
@@ -2165,7 +2164,7 @@
         <v>// U39</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>1</v>
       </c>
@@ -2206,7 +2205,7 @@
         <v>// V0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>3</v>
       </c>
@@ -2247,7 +2246,7 @@
         <v>// V1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>1</v>
       </c>
@@ -2288,7 +2287,7 @@
         <v>// V2</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>3</v>
       </c>
@@ -2329,7 +2328,7 @@
         <v>// V3</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>1</v>
       </c>
@@ -2370,7 +2369,7 @@
         <v>// V4</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>3</v>
       </c>
@@ -2411,7 +2410,7 @@
         <v>// V5</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>1</v>
       </c>
@@ -2452,7 +2451,7 @@
         <v>// V6</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>3</v>
       </c>
@@ -2493,7 +2492,7 @@
         <v>// V7</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>1</v>
       </c>
@@ -2534,7 +2533,7 @@
         <v>// V8</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>3</v>
       </c>
@@ -2575,7 +2574,7 @@
         <v>// V9</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>0</v>
       </c>
@@ -2616,7 +2615,7 @@
         <v>// V10</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>2</v>
       </c>
@@ -2657,7 +2656,7 @@
         <v>// V11</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>0</v>
       </c>
@@ -2698,7 +2697,7 @@
         <v>// V12</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>2</v>
       </c>
@@ -2739,7 +2738,7 @@
         <v>// V13</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>0</v>
       </c>
@@ -2780,7 +2779,7 @@
         <v>// V14</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>2</v>
       </c>
@@ -2821,7 +2820,7 @@
         <v>// V15</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>0</v>
       </c>
@@ -2862,7 +2861,7 @@
         <v>// V16</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>2</v>
       </c>
@@ -2903,7 +2902,7 @@
         <v>// V17</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>0</v>
       </c>
@@ -2944,7 +2943,7 @@
         <v>// V18</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>2</v>
       </c>
@@ -2985,7 +2984,7 @@
         <v>// V19</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>4</v>
       </c>
@@ -3026,7 +3025,7 @@
         <v>// V20</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>6</v>
       </c>
@@ -3067,7 +3066,7 @@
         <v>// V21</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>4</v>
       </c>
@@ -3108,7 +3107,7 @@
         <v>// V22</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>6</v>
       </c>
@@ -3149,7 +3148,7 @@
         <v>// V23</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>4</v>
       </c>
@@ -3190,7 +3189,7 @@
         <v>// V24</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>6</v>
       </c>
@@ -3231,7 +3230,7 @@
         <v>// V25</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>4</v>
       </c>
@@ -3272,7 +3271,7 @@
         <v>// V26</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>6</v>
       </c>
@@ -3313,7 +3312,7 @@
         <v>// V27</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>4</v>
       </c>
@@ -3354,7 +3353,7 @@
         <v>// V28</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>6</v>
       </c>
@@ -3395,7 +3394,7 @@
         <v>// V29</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>5</v>
       </c>
@@ -3436,7 +3435,7 @@
         <v>// V30</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>7</v>
       </c>
@@ -3477,7 +3476,7 @@
         <v>// V31</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>5</v>
       </c>
@@ -3518,7 +3517,7 @@
         <v>// V32</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>7</v>
       </c>
@@ -3559,7 +3558,7 @@
         <v>// V33</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>5</v>
       </c>
@@ -3600,7 +3599,7 @@
         <v>// V34</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>7</v>
       </c>
@@ -3641,7 +3640,7 @@
         <v>// V35</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>5</v>
       </c>
@@ -3682,7 +3681,7 @@
         <v>// V36</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>7</v>
       </c>
@@ -3723,7 +3722,7 @@
         <v>// V37</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>5</v>
       </c>
@@ -3764,7 +3763,7 @@
         <v>// V38</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>7</v>
       </c>
@@ -3805,7 +3804,7 @@
         <v>// V39</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>1</v>
       </c>
@@ -3846,7 +3845,7 @@
         <v>// X0</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>3</v>
       </c>
@@ -3887,7 +3886,7 @@
         <v>// X1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>1</v>
       </c>
@@ -3928,7 +3927,7 @@
         <v>// X2</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>3</v>
       </c>
@@ -3969,7 +3968,7 @@
         <v>// X3</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>1</v>
       </c>
@@ -4010,7 +4009,7 @@
         <v>// X4</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>3</v>
       </c>
@@ -4051,7 +4050,7 @@
         <v>// X5</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>1</v>
       </c>
@@ -4092,7 +4091,7 @@
         <v>// X6</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>3</v>
       </c>
@@ -4133,7 +4132,7 @@
         <v>// X7</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>1</v>
       </c>
@@ -4174,7 +4173,7 @@
         <v>// X8</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>3</v>
       </c>
@@ -4215,7 +4214,7 @@
         <v>// X9</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>1</v>
       </c>
@@ -4256,7 +4255,7 @@
         <v>// X10</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>3</v>
       </c>
@@ -4297,7 +4296,7 @@
         <v>// X11</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>0</v>
       </c>
@@ -4338,7 +4337,7 @@
         <v>// X12</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>2</v>
       </c>
@@ -4379,7 +4378,7 @@
         <v>// X13</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>0</v>
       </c>
@@ -4420,7 +4419,7 @@
         <v>// X14</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>2</v>
       </c>
@@ -4461,7 +4460,7 @@
         <v>// X15</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>0</v>
       </c>
@@ -4502,7 +4501,7 @@
         <v>// X16</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>2</v>
       </c>
@@ -4543,7 +4542,7 @@
         <v>// X17</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>0</v>
       </c>
@@ -4584,7 +4583,7 @@
         <v>// X18</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>2</v>
       </c>
@@ -4625,7 +4624,7 @@
         <v>// X19</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>0</v>
       </c>
@@ -4666,7 +4665,7 @@
         <v>// X20</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>2</v>
       </c>
@@ -4707,7 +4706,7 @@
         <v>// X21</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>0</v>
       </c>
@@ -4748,7 +4747,7 @@
         <v>// X22</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>2</v>
       </c>
@@ -4789,7 +4788,7 @@
         <v>// X23</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>4</v>
       </c>
@@ -4830,7 +4829,7 @@
         <v>// X24</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>6</v>
       </c>
@@ -4871,7 +4870,7 @@
         <v>// X25</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>4</v>
       </c>
@@ -4912,7 +4911,7 @@
         <v>// X26</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>6</v>
       </c>
@@ -4953,7 +4952,7 @@
         <v>// X27</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>4</v>
       </c>
@@ -4994,7 +4993,7 @@
         <v>// X28</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>6</v>
       </c>
@@ -5035,7 +5034,7 @@
         <v>// X29</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>4</v>
       </c>
@@ -5076,7 +5075,7 @@
         <v>// X30</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>6</v>
       </c>
@@ -5117,7 +5116,7 @@
         <v>// X31</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>4</v>
       </c>
@@ -5158,7 +5157,7 @@
         <v>// X32</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>6</v>
       </c>
@@ -5199,7 +5198,7 @@
         <v>// X33</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>4</v>
       </c>
@@ -5240,7 +5239,7 @@
         <v>// X34</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>6</v>
       </c>
@@ -5281,7 +5280,7 @@
         <v>// X35</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>5</v>
       </c>
@@ -5322,7 +5321,7 @@
         <v>// X36</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>7</v>
       </c>
@@ -5363,7 +5362,7 @@
         <v>// X37</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>5</v>
       </c>
@@ -5404,7 +5403,7 @@
         <v>// X38</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>7</v>
       </c>
@@ -5445,7 +5444,7 @@
         <v>// X39</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>5</v>
       </c>
@@ -5486,7 +5485,7 @@
         <v>// X40</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>7</v>
       </c>
@@ -5527,7 +5526,7 @@
         <v>// X41</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>5</v>
       </c>
@@ -5568,7 +5567,7 @@
         <v>// X42</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>7</v>
       </c>
@@ -5609,7 +5608,7 @@
         <v>// X43</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>5</v>
       </c>
@@ -5650,7 +5649,7 @@
         <v>// X44</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>7</v>
       </c>
@@ -5691,7 +5690,7 @@
         <v>// X45</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>5</v>
       </c>
@@ -5732,7 +5731,7 @@
         <v>// X46</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>7</v>
       </c>
@@ -5774,7 +5773,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K129">
+  <sortState ref="A2:K129">
     <sortCondition ref="C2:C129"/>
     <sortCondition ref="D2:D129"/>
   </sortState>
@@ -5783,27 +5782,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14ED0397-3C93-4907-A545-7BA9F176BB22}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N129"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="8.83203125" style="1"/>
-    <col min="9" max="11" width="8.83203125" style="1"/>
-    <col min="12" max="12" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8.875" style="1"/>
+    <col min="9" max="11" width="8.875" style="1"/>
+    <col min="12" max="12" width="14.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -5847,7 +5846,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5898,7 +5897,7 @@
         <v>// U0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5949,7 +5948,7 @@
         <v>// U1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -6000,7 +5999,7 @@
         <v>// U2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -6051,7 +6050,7 @@
         <v>// U3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -6102,7 +6101,7 @@
         <v>// U4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -6153,7 +6152,7 @@
         <v>// U5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -6204,7 +6203,7 @@
         <v>// U6</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -6255,7 +6254,7 @@
         <v>// U7</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C10" s="1">
         <v>1</v>
       </c>
@@ -6300,7 +6299,7 @@
         <v>// U8</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C11" s="1">
         <v>3</v>
       </c>
@@ -6345,7 +6344,7 @@
         <v>// U9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C12" s="1">
         <v>0</v>
       </c>
@@ -6390,7 +6389,7 @@
         <v>// U10</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C13" s="1">
         <v>2</v>
       </c>
@@ -6435,7 +6434,7 @@
         <v>// U11</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C14" s="1">
         <v>0</v>
       </c>
@@ -6480,7 +6479,7 @@
         <v>// U12</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C15" s="1">
         <v>2</v>
       </c>
@@ -6525,7 +6524,7 @@
         <v>// U13</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C16" s="1">
         <v>0</v>
       </c>
@@ -6570,7 +6569,7 @@
         <v>// U14</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C17" s="1">
         <v>2</v>
       </c>
@@ -6615,7 +6614,7 @@
         <v>// U15</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C18" s="1">
         <v>0</v>
       </c>
@@ -6660,7 +6659,7 @@
         <v>// U16</v>
       </c>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C19" s="1">
         <v>2</v>
       </c>
@@ -6705,7 +6704,7 @@
         <v>// U17</v>
       </c>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C20" s="1">
         <v>0</v>
       </c>
@@ -6750,7 +6749,7 @@
         <v>// U18</v>
       </c>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="21" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C21" s="1">
         <v>2</v>
       </c>
@@ -6795,7 +6794,7 @@
         <v>// U19</v>
       </c>
     </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="22" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C22" s="1">
         <v>4</v>
       </c>
@@ -6840,7 +6839,7 @@
         <v>// U20</v>
       </c>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C23" s="1">
         <v>6</v>
       </c>
@@ -6885,7 +6884,7 @@
         <v>// U21</v>
       </c>
     </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="24" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C24" s="1">
         <v>4</v>
       </c>
@@ -6930,7 +6929,7 @@
         <v>// U22</v>
       </c>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="25" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C25" s="1">
         <v>6</v>
       </c>
@@ -6975,7 +6974,7 @@
         <v>// U23</v>
       </c>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C26" s="1">
         <v>4</v>
       </c>
@@ -7020,7 +7019,7 @@
         <v>// U24</v>
       </c>
     </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C27" s="1">
         <v>6</v>
       </c>
@@ -7065,7 +7064,7 @@
         <v>// U25</v>
       </c>
     </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C28" s="1">
         <v>4</v>
       </c>
@@ -7110,7 +7109,7 @@
         <v>// U26</v>
       </c>
     </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="29" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C29" s="1">
         <v>6</v>
       </c>
@@ -7155,7 +7154,7 @@
         <v>// U27</v>
       </c>
     </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="30" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C30" s="1">
         <v>4</v>
       </c>
@@ -7200,7 +7199,7 @@
         <v>// U28</v>
       </c>
     </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C31" s="1">
         <v>6</v>
       </c>
@@ -7245,7 +7244,7 @@
         <v>// U29</v>
       </c>
     </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="32" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C32" s="1">
         <v>5</v>
       </c>
@@ -7290,7 +7289,7 @@
         <v>// U30</v>
       </c>
     </row>
-    <row r="33" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="33" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C33" s="1">
         <v>7</v>
       </c>
@@ -7335,7 +7334,7 @@
         <v>// U31</v>
       </c>
     </row>
-    <row r="34" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="34" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C34" s="1">
         <v>5</v>
       </c>
@@ -7380,7 +7379,7 @@
         <v>// U32</v>
       </c>
     </row>
-    <row r="35" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="35" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C35" s="1">
         <v>7</v>
       </c>
@@ -7425,7 +7424,7 @@
         <v>// U33</v>
       </c>
     </row>
-    <row r="36" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="36" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C36" s="1">
         <v>5</v>
       </c>
@@ -7470,7 +7469,7 @@
         <v>// U34</v>
       </c>
     </row>
-    <row r="37" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="37" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C37" s="1">
         <v>7</v>
       </c>
@@ -7515,7 +7514,7 @@
         <v>// U35</v>
       </c>
     </row>
-    <row r="38" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="38" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C38" s="1">
         <v>5</v>
       </c>
@@ -7560,7 +7559,7 @@
         <v>// U36</v>
       </c>
     </row>
-    <row r="39" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="39" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C39" s="1">
         <v>7</v>
       </c>
@@ -7605,7 +7604,7 @@
         <v>// U37</v>
       </c>
     </row>
-    <row r="40" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="40" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C40" s="1">
         <v>5</v>
       </c>
@@ -7650,7 +7649,7 @@
         <v>// U38</v>
       </c>
     </row>
-    <row r="41" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="41" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C41" s="1">
         <v>7</v>
       </c>
@@ -7695,7 +7694,7 @@
         <v>// U39</v>
       </c>
     </row>
-    <row r="42" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="42" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C42" s="1">
         <v>1</v>
       </c>
@@ -7740,7 +7739,7 @@
         <v>// V0</v>
       </c>
     </row>
-    <row r="43" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="43" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C43" s="1">
         <v>3</v>
       </c>
@@ -7785,7 +7784,7 @@
         <v>// V1</v>
       </c>
     </row>
-    <row r="44" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="44" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C44" s="1">
         <v>1</v>
       </c>
@@ -7830,7 +7829,7 @@
         <v>// V2</v>
       </c>
     </row>
-    <row r="45" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="45" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C45" s="1">
         <v>3</v>
       </c>
@@ -7875,7 +7874,7 @@
         <v>// V3</v>
       </c>
     </row>
-    <row r="46" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="46" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C46" s="1">
         <v>1</v>
       </c>
@@ -7920,7 +7919,7 @@
         <v>// V4</v>
       </c>
     </row>
-    <row r="47" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="47" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C47" s="1">
         <v>3</v>
       </c>
@@ -7965,7 +7964,7 @@
         <v>// V5</v>
       </c>
     </row>
-    <row r="48" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="48" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C48" s="1">
         <v>1</v>
       </c>
@@ -8010,7 +8009,7 @@
         <v>// V6</v>
       </c>
     </row>
-    <row r="49" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="49" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C49" s="1">
         <v>3</v>
       </c>
@@ -8055,7 +8054,7 @@
         <v>// V7</v>
       </c>
     </row>
-    <row r="50" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="50" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C50" s="1">
         <v>1</v>
       </c>
@@ -8100,7 +8099,7 @@
         <v>// V8</v>
       </c>
     </row>
-    <row r="51" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="51" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C51" s="1">
         <v>3</v>
       </c>
@@ -8145,7 +8144,7 @@
         <v>// V9</v>
       </c>
     </row>
-    <row r="52" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="52" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C52" s="1">
         <v>0</v>
       </c>
@@ -8190,7 +8189,7 @@
         <v>// V10</v>
       </c>
     </row>
-    <row r="53" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="53" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C53" s="1">
         <v>2</v>
       </c>
@@ -8235,7 +8234,7 @@
         <v>// V11</v>
       </c>
     </row>
-    <row r="54" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="54" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C54" s="1">
         <v>0</v>
       </c>
@@ -8280,7 +8279,7 @@
         <v>// V12</v>
       </c>
     </row>
-    <row r="55" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="55" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C55" s="1">
         <v>2</v>
       </c>
@@ -8325,7 +8324,7 @@
         <v>// V13</v>
       </c>
     </row>
-    <row r="56" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="56" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C56" s="1">
         <v>0</v>
       </c>
@@ -8370,7 +8369,7 @@
         <v>// V14</v>
       </c>
     </row>
-    <row r="57" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="57" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C57" s="1">
         <v>2</v>
       </c>
@@ -8415,7 +8414,7 @@
         <v>// V15</v>
       </c>
     </row>
-    <row r="58" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="58" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C58" s="1">
         <v>0</v>
       </c>
@@ -8460,7 +8459,7 @@
         <v>// V16</v>
       </c>
     </row>
-    <row r="59" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="59" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C59" s="1">
         <v>2</v>
       </c>
@@ -8505,7 +8504,7 @@
         <v>// V17</v>
       </c>
     </row>
-    <row r="60" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="60" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C60" s="1">
         <v>0</v>
       </c>
@@ -8550,7 +8549,7 @@
         <v>// V18</v>
       </c>
     </row>
-    <row r="61" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="61" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C61" s="1">
         <v>2</v>
       </c>
@@ -8595,7 +8594,7 @@
         <v>// V19</v>
       </c>
     </row>
-    <row r="62" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="62" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C62" s="1">
         <v>4</v>
       </c>
@@ -8640,7 +8639,7 @@
         <v>// V20</v>
       </c>
     </row>
-    <row r="63" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="63" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C63" s="1">
         <v>6</v>
       </c>
@@ -8685,7 +8684,7 @@
         <v>// V21</v>
       </c>
     </row>
-    <row r="64" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="64" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C64" s="1">
         <v>4</v>
       </c>
@@ -8730,7 +8729,7 @@
         <v>// V22</v>
       </c>
     </row>
-    <row r="65" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="65" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C65" s="1">
         <v>6</v>
       </c>
@@ -8775,7 +8774,7 @@
         <v>// V23</v>
       </c>
     </row>
-    <row r="66" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="66" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C66" s="1">
         <v>4</v>
       </c>
@@ -8820,7 +8819,7 @@
         <v>// V24</v>
       </c>
     </row>
-    <row r="67" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="67" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C67" s="1">
         <v>6</v>
       </c>
@@ -8865,7 +8864,7 @@
         <v>// V25</v>
       </c>
     </row>
-    <row r="68" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="68" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C68" s="1">
         <v>4</v>
       </c>
@@ -8910,7 +8909,7 @@
         <v>// V26</v>
       </c>
     </row>
-    <row r="69" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="69" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C69" s="1">
         <v>6</v>
       </c>
@@ -8955,7 +8954,7 @@
         <v>// V27</v>
       </c>
     </row>
-    <row r="70" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="70" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C70" s="1">
         <v>4</v>
       </c>
@@ -9000,7 +8999,7 @@
         <v>// V28</v>
       </c>
     </row>
-    <row r="71" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="71" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C71" s="1">
         <v>6</v>
       </c>
@@ -9045,7 +9044,7 @@
         <v>// V29</v>
       </c>
     </row>
-    <row r="72" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="72" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C72" s="1">
         <v>5</v>
       </c>
@@ -9090,7 +9089,7 @@
         <v>// V30</v>
       </c>
     </row>
-    <row r="73" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="73" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C73" s="1">
         <v>7</v>
       </c>
@@ -9135,7 +9134,7 @@
         <v>// V31</v>
       </c>
     </row>
-    <row r="74" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="74" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C74" s="1">
         <v>5</v>
       </c>
@@ -9180,7 +9179,7 @@
         <v>// V32</v>
       </c>
     </row>
-    <row r="75" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="75" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C75" s="1">
         <v>7</v>
       </c>
@@ -9225,7 +9224,7 @@
         <v>// V33</v>
       </c>
     </row>
-    <row r="76" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="76" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C76" s="1">
         <v>5</v>
       </c>
@@ -9270,7 +9269,7 @@
         <v>// V34</v>
       </c>
     </row>
-    <row r="77" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="77" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C77" s="1">
         <v>7</v>
       </c>
@@ -9315,7 +9314,7 @@
         <v>// V35</v>
       </c>
     </row>
-    <row r="78" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="78" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C78" s="1">
         <v>5</v>
       </c>
@@ -9360,7 +9359,7 @@
         <v>// V36</v>
       </c>
     </row>
-    <row r="79" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="79" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C79" s="1">
         <v>7</v>
       </c>
@@ -9405,7 +9404,7 @@
         <v>// V37</v>
       </c>
     </row>
-    <row r="80" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="80" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C80" s="1">
         <v>5</v>
       </c>
@@ -9450,7 +9449,7 @@
         <v>// V38</v>
       </c>
     </row>
-    <row r="81" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="81" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C81" s="1">
         <v>7</v>
       </c>
@@ -9495,7 +9494,7 @@
         <v>// V39</v>
       </c>
     </row>
-    <row r="82" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="82" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C82" s="1">
         <v>1</v>
       </c>
@@ -9540,7 +9539,7 @@
         <v>// X0</v>
       </c>
     </row>
-    <row r="83" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="83" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C83" s="1">
         <v>3</v>
       </c>
@@ -9585,7 +9584,7 @@
         <v>// X1</v>
       </c>
     </row>
-    <row r="84" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="84" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C84" s="1">
         <v>1</v>
       </c>
@@ -9630,7 +9629,7 @@
         <v>// X2</v>
       </c>
     </row>
-    <row r="85" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="85" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C85" s="1">
         <v>3</v>
       </c>
@@ -9675,7 +9674,7 @@
         <v>// X3</v>
       </c>
     </row>
-    <row r="86" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="86" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C86" s="1">
         <v>1</v>
       </c>
@@ -9720,7 +9719,7 @@
         <v>// X4</v>
       </c>
     </row>
-    <row r="87" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="87" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C87" s="1">
         <v>3</v>
       </c>
@@ -9765,7 +9764,7 @@
         <v>// X5</v>
       </c>
     </row>
-    <row r="88" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="88" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C88" s="1">
         <v>1</v>
       </c>
@@ -9810,7 +9809,7 @@
         <v>// X6</v>
       </c>
     </row>
-    <row r="89" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="89" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C89" s="1">
         <v>3</v>
       </c>
@@ -9855,7 +9854,7 @@
         <v>// X7</v>
       </c>
     </row>
-    <row r="90" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="90" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C90" s="1">
         <v>1</v>
       </c>
@@ -9900,7 +9899,7 @@
         <v>// X8</v>
       </c>
     </row>
-    <row r="91" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="91" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C91" s="1">
         <v>3</v>
       </c>
@@ -9945,7 +9944,7 @@
         <v>// X9</v>
       </c>
     </row>
-    <row r="92" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="92" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C92" s="1">
         <v>1</v>
       </c>
@@ -9990,7 +9989,7 @@
         <v>// X10</v>
       </c>
     </row>
-    <row r="93" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="93" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C93" s="1">
         <v>3</v>
       </c>
@@ -10035,7 +10034,7 @@
         <v>// X11</v>
       </c>
     </row>
-    <row r="94" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="94" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C94" s="1">
         <v>0</v>
       </c>
@@ -10080,7 +10079,7 @@
         <v>// X12</v>
       </c>
     </row>
-    <row r="95" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="95" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C95" s="1">
         <v>2</v>
       </c>
@@ -10125,7 +10124,7 @@
         <v>// X13</v>
       </c>
     </row>
-    <row r="96" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="96" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C96" s="1">
         <v>0</v>
       </c>
@@ -10170,7 +10169,7 @@
         <v>// X14</v>
       </c>
     </row>
-    <row r="97" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="97" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C97" s="1">
         <v>2</v>
       </c>
@@ -10215,7 +10214,7 @@
         <v>// X15</v>
       </c>
     </row>
-    <row r="98" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="98" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C98" s="1">
         <v>0</v>
       </c>
@@ -10260,7 +10259,7 @@
         <v>// X16</v>
       </c>
     </row>
-    <row r="99" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="99" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C99" s="1">
         <v>2</v>
       </c>
@@ -10305,7 +10304,7 @@
         <v>// X17</v>
       </c>
     </row>
-    <row r="100" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="100" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C100" s="1">
         <v>0</v>
       </c>
@@ -10350,7 +10349,7 @@
         <v>// X18</v>
       </c>
     </row>
-    <row r="101" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="101" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C101" s="1">
         <v>2</v>
       </c>
@@ -10395,7 +10394,7 @@
         <v>// X19</v>
       </c>
     </row>
-    <row r="102" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="102" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C102" s="1">
         <v>0</v>
       </c>
@@ -10440,7 +10439,7 @@
         <v>// X20</v>
       </c>
     </row>
-    <row r="103" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="103" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C103" s="1">
         <v>2</v>
       </c>
@@ -10485,7 +10484,7 @@
         <v>// X21</v>
       </c>
     </row>
-    <row r="104" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="104" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C104" s="1">
         <v>0</v>
       </c>
@@ -10530,7 +10529,7 @@
         <v>// X22</v>
       </c>
     </row>
-    <row r="105" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="105" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C105" s="1">
         <v>2</v>
       </c>
@@ -10575,7 +10574,7 @@
         <v>// X23</v>
       </c>
     </row>
-    <row r="106" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="106" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C106" s="1">
         <v>4</v>
       </c>
@@ -10620,7 +10619,7 @@
         <v>// X24</v>
       </c>
     </row>
-    <row r="107" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="107" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C107" s="1">
         <v>6</v>
       </c>
@@ -10665,7 +10664,7 @@
         <v>// X25</v>
       </c>
     </row>
-    <row r="108" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="108" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C108" s="1">
         <v>4</v>
       </c>
@@ -10710,7 +10709,7 @@
         <v>// X26</v>
       </c>
     </row>
-    <row r="109" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="109" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C109" s="1">
         <v>6</v>
       </c>
@@ -10755,7 +10754,7 @@
         <v>// X27</v>
       </c>
     </row>
-    <row r="110" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="110" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C110" s="1">
         <v>4</v>
       </c>
@@ -10800,7 +10799,7 @@
         <v>// X28</v>
       </c>
     </row>
-    <row r="111" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="111" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C111" s="1">
         <v>6</v>
       </c>
@@ -10845,7 +10844,7 @@
         <v>// X29</v>
       </c>
     </row>
-    <row r="112" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="112" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C112" s="1">
         <v>4</v>
       </c>
@@ -10890,7 +10889,7 @@
         <v>// X30</v>
       </c>
     </row>
-    <row r="113" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="113" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C113" s="1">
         <v>6</v>
       </c>
@@ -10935,7 +10934,7 @@
         <v>// X31</v>
       </c>
     </row>
-    <row r="114" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="114" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C114" s="1">
         <v>4</v>
       </c>
@@ -10980,7 +10979,7 @@
         <v>// X32</v>
       </c>
     </row>
-    <row r="115" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="115" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C115" s="1">
         <v>6</v>
       </c>
@@ -11025,7 +11024,7 @@
         <v>// X33</v>
       </c>
     </row>
-    <row r="116" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="116" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C116" s="1">
         <v>4</v>
       </c>
@@ -11070,7 +11069,7 @@
         <v>// X34</v>
       </c>
     </row>
-    <row r="117" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="117" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C117" s="1">
         <v>6</v>
       </c>
@@ -11115,7 +11114,7 @@
         <v>// X35</v>
       </c>
     </row>
-    <row r="118" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="118" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C118" s="1">
         <v>5</v>
       </c>
@@ -11160,7 +11159,7 @@
         <v>// X36</v>
       </c>
     </row>
-    <row r="119" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="119" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C119" s="1">
         <v>7</v>
       </c>
@@ -11205,7 +11204,7 @@
         <v>// X37</v>
       </c>
     </row>
-    <row r="120" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="120" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C120" s="1">
         <v>5</v>
       </c>
@@ -11250,7 +11249,7 @@
         <v>// X38</v>
       </c>
     </row>
-    <row r="121" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="121" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C121" s="1">
         <v>7</v>
       </c>
@@ -11295,7 +11294,7 @@
         <v>// X39</v>
       </c>
     </row>
-    <row r="122" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="122" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C122" s="1">
         <v>5</v>
       </c>
@@ -11340,7 +11339,7 @@
         <v>// X40</v>
       </c>
     </row>
-    <row r="123" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="123" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C123" s="1">
         <v>7</v>
       </c>
@@ -11385,7 +11384,7 @@
         <v>// X41</v>
       </c>
     </row>
-    <row r="124" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="124" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C124" s="1">
         <v>5</v>
       </c>
@@ -11430,7 +11429,7 @@
         <v>// X42</v>
       </c>
     </row>
-    <row r="125" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="125" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C125" s="1">
         <v>7</v>
       </c>
@@ -11475,7 +11474,7 @@
         <v>// X43</v>
       </c>
     </row>
-    <row r="126" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="126" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C126" s="1">
         <v>5</v>
       </c>
@@ -11520,7 +11519,7 @@
         <v>// X44</v>
       </c>
     </row>
-    <row r="127" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="127" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C127" s="1">
         <v>7</v>
       </c>
@@ -11565,7 +11564,7 @@
         <v>// X45</v>
       </c>
     </row>
-    <row r="128" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="128" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C128" s="1">
         <v>5</v>
       </c>
@@ -11610,7 +11609,7 @@
         <v>// X46</v>
       </c>
     </row>
-    <row r="129" spans="3:14" x14ac:dyDescent="0.15">
+    <row r="129" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C129" s="1">
         <v>7</v>
       </c>
@@ -11656,7 +11655,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B9">
+  <sortState ref="A2:B9">
     <sortCondition ref="A2:A9"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11664,23 +11663,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA75860-87A9-9347-B3C0-A1426EC2A64A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J129"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J66" sqref="J66:J129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="8.83203125" style="1"/>
-    <col min="6" max="8" width="8.83203125" style="1"/>
-    <col min="9" max="9" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="54.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="8.875" style="1"/>
+    <col min="6" max="8" width="8.875" style="1"/>
+    <col min="9" max="9" width="14.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="54.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11715,7 +11714,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -11756,7 +11755,7 @@
         <v>// U18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -11797,7 +11796,7 @@
         <v>// U16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -11838,7 +11837,7 @@
         <v>// U14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -11879,7 +11878,7 @@
         <v>// U12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -11920,7 +11919,7 @@
         <v>// U10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -11961,7 +11960,7 @@
         <v>// V18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -12002,7 +12001,7 @@
         <v>// V16</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -12043,7 +12042,7 @@
         <v>// V14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -12084,7 +12083,7 @@
         <v>// V12</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -12125,7 +12124,7 @@
         <v>// V10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -12166,7 +12165,7 @@
         <v>// X22</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -12207,7 +12206,7 @@
         <v>// X20</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -12248,7 +12247,7 @@
         <v>// X18</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -12289,7 +12288,7 @@
         <v>// X16</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -12330,7 +12329,7 @@
         <v>// X14</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -12371,7 +12370,7 @@
         <v>// X12</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -12412,7 +12411,7 @@
         <v>// U8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -12453,7 +12452,7 @@
         <v>// U6</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -12494,7 +12493,7 @@
         <v>// U4</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -12535,7 +12534,7 @@
         <v>// U2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -12576,7 +12575,7 @@
         <v>// U0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -12617,7 +12616,7 @@
         <v>// V8</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -12658,7 +12657,7 @@
         <v>// V6</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -12699,7 +12698,7 @@
         <v>// V4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -12740,7 +12739,7 @@
         <v>// V2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -12781,7 +12780,7 @@
         <v>// V0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -12822,7 +12821,7 @@
         <v>// X10</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -12863,7 +12862,7 @@
         <v>// X8</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -12904,7 +12903,7 @@
         <v>// X6</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -12945,7 +12944,7 @@
         <v>// X4</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -12986,7 +12985,7 @@
         <v>// X2</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>1</v>
       </c>
@@ -13027,7 +13026,7 @@
         <v>// X0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>2</v>
       </c>
@@ -13068,7 +13067,7 @@
         <v>// X13</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>2</v>
       </c>
@@ -13109,7 +13108,7 @@
         <v>// X15</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>2</v>
       </c>
@@ -13150,7 +13149,7 @@
         <v>// X17</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2</v>
       </c>
@@ -13191,7 +13190,7 @@
         <v>// X19</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2</v>
       </c>
@@ -13232,7 +13231,7 @@
         <v>// X21</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2</v>
       </c>
@@ -13273,7 +13272,7 @@
         <v>// X23</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2</v>
       </c>
@@ -13314,7 +13313,7 @@
         <v>// V11</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2</v>
       </c>
@@ -13355,7 +13354,7 @@
         <v>// V13</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2</v>
       </c>
@@ -13396,7 +13395,7 @@
         <v>// V15</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2</v>
       </c>
@@ -13437,7 +13436,7 @@
         <v>// V17</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>2</v>
       </c>
@@ -13478,7 +13477,7 @@
         <v>// V19</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>2</v>
       </c>
@@ -13519,7 +13518,7 @@
         <v>// U11</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>2</v>
       </c>
@@ -13560,7 +13559,7 @@
         <v>// U13</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>2</v>
       </c>
@@ -13601,7 +13600,7 @@
         <v>// U15</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>2</v>
       </c>
@@ -13642,7 +13641,7 @@
         <v>// U17</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2</v>
       </c>
@@ -13683,7 +13682,7 @@
         <v>// U19</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>3</v>
       </c>
@@ -13724,7 +13723,7 @@
         <v>// X1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>3</v>
       </c>
@@ -13765,7 +13764,7 @@
         <v>// X3</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>3</v>
       </c>
@@ -13806,7 +13805,7 @@
         <v>// X5</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>3</v>
       </c>
@@ -13847,7 +13846,7 @@
         <v>// X7</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>3</v>
       </c>
@@ -13888,7 +13887,7 @@
         <v>// X9</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>3</v>
       </c>
@@ -13929,7 +13928,7 @@
         <v>// X11</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>3</v>
       </c>
@@ -13970,7 +13969,7 @@
         <v>// V1</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>3</v>
       </c>
@@ -14011,7 +14010,7 @@
         <v>// V3</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>3</v>
       </c>
@@ -14052,7 +14051,7 @@
         <v>// V5</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>3</v>
       </c>
@@ -14093,7 +14092,7 @@
         <v>// V7</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>3</v>
       </c>
@@ -14134,7 +14133,7 @@
         <v>// V9</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>3</v>
       </c>
@@ -14175,7 +14174,7 @@
         <v>// U1</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>3</v>
       </c>
@@ -14216,7 +14215,7 @@
         <v>// U3</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>3</v>
       </c>
@@ -14257,7 +14256,7 @@
         <v>// U5</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>3</v>
       </c>
@@ -14298,7 +14297,7 @@
         <v>// U7</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>3</v>
       </c>
@@ -14339,7 +14338,7 @@
         <v>// U9</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>4</v>
       </c>
@@ -14372,15 +14371,15 @@
         <v>0</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">            parallel_daq_0 [0 +: 14] = deframed_mapped [1][0][0];</v>
+        <f>CONCATENATE("            parallel_daq_1 [",F66," +: 14] = deframed_mapped [",H66,"][",I66,"][",B66,"];")</f>
+        <v xml:space="preserve">            parallel_daq_1 [0 +: 14] = deframed_mapped [1][0][0];</v>
       </c>
       <c r="K66" t="str">
         <f t="shared" ref="K66:K129" si="10">CONCATENATE("// ",C66,D66)</f>
         <v>// U28</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>4</v>
       </c>
@@ -14413,15 +14412,15 @@
         <v>0</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" ref="J67:J129" si="11">CONCATENATE("            parallel_daq_0 [",F67," +: 14] = deframed_mapped [",H67,"][",I67,"][",B67,"];")</f>
-        <v xml:space="preserve">            parallel_daq_0 [14 +: 14] = deframed_mapped [1][0][1];</v>
+        <f t="shared" ref="J67:J129" si="11">CONCATENATE("            parallel_daq_1 [",F67," +: 14] = deframed_mapped [",H67,"][",I67,"][",B67,"];")</f>
+        <v xml:space="preserve">            parallel_daq_1 [14 +: 14] = deframed_mapped [1][0][1];</v>
       </c>
       <c r="K67" t="str">
         <f t="shared" si="10"/>
         <v>// U26</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>4</v>
       </c>
@@ -14455,14 +14454,14 @@
       </c>
       <c r="J68" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [28 +: 14] = deframed_mapped [1][0][2];</v>
+        <v xml:space="preserve">            parallel_daq_1 [28 +: 14] = deframed_mapped [1][0][2];</v>
       </c>
       <c r="K68" t="str">
         <f t="shared" si="10"/>
         <v>// U24</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>4</v>
       </c>
@@ -14496,14 +14495,14 @@
       </c>
       <c r="J69" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [42 +: 14] = deframed_mapped [1][0][3];</v>
+        <v xml:space="preserve">            parallel_daq_1 [42 +: 14] = deframed_mapped [1][0][3];</v>
       </c>
       <c r="K69" t="str">
         <f t="shared" si="10"/>
         <v>// U22</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>4</v>
       </c>
@@ -14537,14 +14536,14 @@
       </c>
       <c r="J70" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [56 +: 14] = deframed_mapped [1][0][4];</v>
+        <v xml:space="preserve">            parallel_daq_1 [56 +: 14] = deframed_mapped [1][0][4];</v>
       </c>
       <c r="K70" t="str">
         <f t="shared" si="10"/>
         <v>// U20</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>4</v>
       </c>
@@ -14578,14 +14577,14 @@
       </c>
       <c r="J71" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [70 +: 14] = deframed_mapped [1][0][5];</v>
+        <v xml:space="preserve">            parallel_daq_1 [70 +: 14] = deframed_mapped [1][0][5];</v>
       </c>
       <c r="K71" t="str">
         <f t="shared" si="10"/>
         <v>// V28</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>4</v>
       </c>
@@ -14619,14 +14618,14 @@
       </c>
       <c r="J72" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [84 +: 14] = deframed_mapped [1][0][6];</v>
+        <v xml:space="preserve">            parallel_daq_1 [84 +: 14] = deframed_mapped [1][0][6];</v>
       </c>
       <c r="K72" t="str">
         <f t="shared" si="10"/>
         <v>// V26</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>4</v>
       </c>
@@ -14660,14 +14659,14 @@
       </c>
       <c r="J73" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [98 +: 14] = deframed_mapped [1][0][7];</v>
+        <v xml:space="preserve">            parallel_daq_1 [98 +: 14] = deframed_mapped [1][0][7];</v>
       </c>
       <c r="K73" t="str">
         <f t="shared" si="10"/>
         <v>// V24</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>4</v>
       </c>
@@ -14701,14 +14700,14 @@
       </c>
       <c r="J74" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [112 +: 14] = deframed_mapped [1][0][8];</v>
+        <v xml:space="preserve">            parallel_daq_1 [112 +: 14] = deframed_mapped [1][0][8];</v>
       </c>
       <c r="K74" t="str">
         <f t="shared" si="10"/>
         <v>// V22</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>4</v>
       </c>
@@ -14742,14 +14741,14 @@
       </c>
       <c r="J75" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [126 +: 14] = deframed_mapped [1][0][9];</v>
+        <v xml:space="preserve">            parallel_daq_1 [126 +: 14] = deframed_mapped [1][0][9];</v>
       </c>
       <c r="K75" t="str">
         <f t="shared" si="10"/>
         <v>// V20</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>4</v>
       </c>
@@ -14783,14 +14782,14 @@
       </c>
       <c r="J76" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [140 +: 14] = deframed_mapped [1][0][10];</v>
+        <v xml:space="preserve">            parallel_daq_1 [140 +: 14] = deframed_mapped [1][0][10];</v>
       </c>
       <c r="K76" t="str">
         <f t="shared" si="10"/>
         <v>// X34</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>4</v>
       </c>
@@ -14824,14 +14823,14 @@
       </c>
       <c r="J77" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [154 +: 14] = deframed_mapped [1][0][11];</v>
+        <v xml:space="preserve">            parallel_daq_1 [154 +: 14] = deframed_mapped [1][0][11];</v>
       </c>
       <c r="K77" t="str">
         <f t="shared" si="10"/>
         <v>// X32</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>4</v>
       </c>
@@ -14865,14 +14864,14 @@
       </c>
       <c r="J78" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [168 +: 14] = deframed_mapped [1][0][12];</v>
+        <v xml:space="preserve">            parallel_daq_1 [168 +: 14] = deframed_mapped [1][0][12];</v>
       </c>
       <c r="K78" t="str">
         <f t="shared" si="10"/>
         <v>// X30</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>4</v>
       </c>
@@ -14906,14 +14905,14 @@
       </c>
       <c r="J79" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [182 +: 14] = deframed_mapped [1][0][13];</v>
+        <v xml:space="preserve">            parallel_daq_1 [182 +: 14] = deframed_mapped [1][0][13];</v>
       </c>
       <c r="K79" t="str">
         <f t="shared" si="10"/>
         <v>// X28</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>4</v>
       </c>
@@ -14947,14 +14946,14 @@
       </c>
       <c r="J80" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [196 +: 14] = deframed_mapped [1][0][14];</v>
+        <v xml:space="preserve">            parallel_daq_1 [196 +: 14] = deframed_mapped [1][0][14];</v>
       </c>
       <c r="K80" t="str">
         <f t="shared" si="10"/>
         <v>// X26</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>4</v>
       </c>
@@ -14988,14 +14987,14 @@
       </c>
       <c r="J81" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [210 +: 14] = deframed_mapped [1][0][15];</v>
+        <v xml:space="preserve">            parallel_daq_1 [210 +: 14] = deframed_mapped [1][0][15];</v>
       </c>
       <c r="K81" t="str">
         <f t="shared" si="10"/>
         <v>// X24</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>5</v>
       </c>
@@ -15029,14 +15028,14 @@
       </c>
       <c r="J82" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [224 +: 14] = deframed_mapped [1][1][0];</v>
+        <v xml:space="preserve">            parallel_daq_1 [224 +: 14] = deframed_mapped [1][1][0];</v>
       </c>
       <c r="K82" t="str">
         <f t="shared" si="10"/>
         <v>// U38</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>5</v>
       </c>
@@ -15070,14 +15069,14 @@
       </c>
       <c r="J83" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [238 +: 14] = deframed_mapped [1][1][1];</v>
+        <v xml:space="preserve">            parallel_daq_1 [238 +: 14] = deframed_mapped [1][1][1];</v>
       </c>
       <c r="K83" t="str">
         <f t="shared" si="10"/>
         <v>// U36</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>5</v>
       </c>
@@ -15111,14 +15110,14 @@
       </c>
       <c r="J84" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [252 +: 14] = deframed_mapped [1][1][2];</v>
+        <v xml:space="preserve">            parallel_daq_1 [252 +: 14] = deframed_mapped [1][1][2];</v>
       </c>
       <c r="K84" t="str">
         <f t="shared" si="10"/>
         <v>// U34</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>5</v>
       </c>
@@ -15152,14 +15151,14 @@
       </c>
       <c r="J85" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [266 +: 14] = deframed_mapped [1][1][3];</v>
+        <v xml:space="preserve">            parallel_daq_1 [266 +: 14] = deframed_mapped [1][1][3];</v>
       </c>
       <c r="K85" t="str">
         <f t="shared" si="10"/>
         <v>// U32</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>5</v>
       </c>
@@ -15193,14 +15192,14 @@
       </c>
       <c r="J86" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [280 +: 14] = deframed_mapped [1][1][4];</v>
+        <v xml:space="preserve">            parallel_daq_1 [280 +: 14] = deframed_mapped [1][1][4];</v>
       </c>
       <c r="K86" t="str">
         <f t="shared" si="10"/>
         <v>// U30</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>5</v>
       </c>
@@ -15234,14 +15233,14 @@
       </c>
       <c r="J87" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [294 +: 14] = deframed_mapped [1][1][5];</v>
+        <v xml:space="preserve">            parallel_daq_1 [294 +: 14] = deframed_mapped [1][1][5];</v>
       </c>
       <c r="K87" t="str">
         <f t="shared" si="10"/>
         <v>// V38</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>5</v>
       </c>
@@ -15275,14 +15274,14 @@
       </c>
       <c r="J88" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [308 +: 14] = deframed_mapped [1][1][6];</v>
+        <v xml:space="preserve">            parallel_daq_1 [308 +: 14] = deframed_mapped [1][1][6];</v>
       </c>
       <c r="K88" t="str">
         <f t="shared" si="10"/>
         <v>// V36</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>5</v>
       </c>
@@ -15316,14 +15315,14 @@
       </c>
       <c r="J89" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [322 +: 14] = deframed_mapped [1][1][7];</v>
+        <v xml:space="preserve">            parallel_daq_1 [322 +: 14] = deframed_mapped [1][1][7];</v>
       </c>
       <c r="K89" t="str">
         <f t="shared" si="10"/>
         <v>// V34</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>5</v>
       </c>
@@ -15357,14 +15356,14 @@
       </c>
       <c r="J90" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [336 +: 14] = deframed_mapped [1][1][8];</v>
+        <v xml:space="preserve">            parallel_daq_1 [336 +: 14] = deframed_mapped [1][1][8];</v>
       </c>
       <c r="K90" t="str">
         <f t="shared" si="10"/>
         <v>// V32</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>5</v>
       </c>
@@ -15398,14 +15397,14 @@
       </c>
       <c r="J91" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [350 +: 14] = deframed_mapped [1][1][9];</v>
+        <v xml:space="preserve">            parallel_daq_1 [350 +: 14] = deframed_mapped [1][1][9];</v>
       </c>
       <c r="K91" t="str">
         <f t="shared" si="10"/>
         <v>// V30</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>5</v>
       </c>
@@ -15439,14 +15438,14 @@
       </c>
       <c r="J92" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [364 +: 14] = deframed_mapped [1][1][10];</v>
+        <v xml:space="preserve">            parallel_daq_1 [364 +: 14] = deframed_mapped [1][1][10];</v>
       </c>
       <c r="K92" t="str">
         <f t="shared" si="10"/>
         <v>// X46</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>5</v>
       </c>
@@ -15480,14 +15479,14 @@
       </c>
       <c r="J93" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [378 +: 14] = deframed_mapped [1][1][11];</v>
+        <v xml:space="preserve">            parallel_daq_1 [378 +: 14] = deframed_mapped [1][1][11];</v>
       </c>
       <c r="K93" t="str">
         <f t="shared" si="10"/>
         <v>// X44</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>5</v>
       </c>
@@ -15521,14 +15520,14 @@
       </c>
       <c r="J94" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [392 +: 14] = deframed_mapped [1][1][12];</v>
+        <v xml:space="preserve">            parallel_daq_1 [392 +: 14] = deframed_mapped [1][1][12];</v>
       </c>
       <c r="K94" t="str">
         <f t="shared" si="10"/>
         <v>// X42</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>5</v>
       </c>
@@ -15562,14 +15561,14 @@
       </c>
       <c r="J95" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [406 +: 14] = deframed_mapped [1][1][13];</v>
+        <v xml:space="preserve">            parallel_daq_1 [406 +: 14] = deframed_mapped [1][1][13];</v>
       </c>
       <c r="K95" t="str">
         <f t="shared" si="10"/>
         <v>// X40</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>5</v>
       </c>
@@ -15603,14 +15602,14 @@
       </c>
       <c r="J96" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [420 +: 14] = deframed_mapped [1][1][14];</v>
+        <v xml:space="preserve">            parallel_daq_1 [420 +: 14] = deframed_mapped [1][1][14];</v>
       </c>
       <c r="K96" t="str">
         <f t="shared" si="10"/>
         <v>// X38</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>5</v>
       </c>
@@ -15644,14 +15643,14 @@
       </c>
       <c r="J97" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [434 +: 14] = deframed_mapped [1][1][15];</v>
+        <v xml:space="preserve">            parallel_daq_1 [434 +: 14] = deframed_mapped [1][1][15];</v>
       </c>
       <c r="K97" t="str">
         <f t="shared" si="10"/>
         <v>// X36</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>6</v>
       </c>
@@ -15685,14 +15684,14 @@
       </c>
       <c r="J98" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [448 +: 14] = deframed_mapped [1][2][0];</v>
+        <v xml:space="preserve">            parallel_daq_1 [448 +: 14] = deframed_mapped [1][2][0];</v>
       </c>
       <c r="K98" t="str">
         <f t="shared" si="10"/>
         <v>// X25</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>6</v>
       </c>
@@ -15726,14 +15725,14 @@
       </c>
       <c r="J99" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [462 +: 14] = deframed_mapped [1][2][1];</v>
+        <v xml:space="preserve">            parallel_daq_1 [462 +: 14] = deframed_mapped [1][2][1];</v>
       </c>
       <c r="K99" t="str">
         <f t="shared" si="10"/>
         <v>// X27</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>6</v>
       </c>
@@ -15767,14 +15766,14 @@
       </c>
       <c r="J100" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [476 +: 14] = deframed_mapped [1][2][2];</v>
+        <v xml:space="preserve">            parallel_daq_1 [476 +: 14] = deframed_mapped [1][2][2];</v>
       </c>
       <c r="K100" t="str">
         <f t="shared" si="10"/>
         <v>// X29</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>6</v>
       </c>
@@ -15808,14 +15807,14 @@
       </c>
       <c r="J101" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [490 +: 14] = deframed_mapped [1][2][3];</v>
+        <v xml:space="preserve">            parallel_daq_1 [490 +: 14] = deframed_mapped [1][2][3];</v>
       </c>
       <c r="K101" t="str">
         <f t="shared" si="10"/>
         <v>// X31</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>6</v>
       </c>
@@ -15849,14 +15848,14 @@
       </c>
       <c r="J102" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [504 +: 14] = deframed_mapped [1][2][4];</v>
+        <v xml:space="preserve">            parallel_daq_1 [504 +: 14] = deframed_mapped [1][2][4];</v>
       </c>
       <c r="K102" t="str">
         <f t="shared" si="10"/>
         <v>// X33</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>6</v>
       </c>
@@ -15890,14 +15889,14 @@
       </c>
       <c r="J103" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [518 +: 14] = deframed_mapped [1][2][5];</v>
+        <v xml:space="preserve">            parallel_daq_1 [518 +: 14] = deframed_mapped [1][2][5];</v>
       </c>
       <c r="K103" t="str">
         <f t="shared" si="10"/>
         <v>// X35</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>6</v>
       </c>
@@ -15931,14 +15930,14 @@
       </c>
       <c r="J104" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [532 +: 14] = deframed_mapped [1][2][6];</v>
+        <v xml:space="preserve">            parallel_daq_1 [532 +: 14] = deframed_mapped [1][2][6];</v>
       </c>
       <c r="K104" t="str">
         <f t="shared" si="10"/>
         <v>// V21</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>6</v>
       </c>
@@ -15972,14 +15971,14 @@
       </c>
       <c r="J105" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [546 +: 14] = deframed_mapped [1][2][7];</v>
+        <v xml:space="preserve">            parallel_daq_1 [546 +: 14] = deframed_mapped [1][2][7];</v>
       </c>
       <c r="K105" t="str">
         <f t="shared" si="10"/>
         <v>// V23</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>6</v>
       </c>
@@ -16013,14 +16012,14 @@
       </c>
       <c r="J106" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [560 +: 14] = deframed_mapped [1][2][8];</v>
+        <v xml:space="preserve">            parallel_daq_1 [560 +: 14] = deframed_mapped [1][2][8];</v>
       </c>
       <c r="K106" t="str">
         <f t="shared" si="10"/>
         <v>// V25</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>6</v>
       </c>
@@ -16054,14 +16053,14 @@
       </c>
       <c r="J107" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [574 +: 14] = deframed_mapped [1][2][9];</v>
+        <v xml:space="preserve">            parallel_daq_1 [574 +: 14] = deframed_mapped [1][2][9];</v>
       </c>
       <c r="K107" t="str">
         <f t="shared" si="10"/>
         <v>// V27</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>6</v>
       </c>
@@ -16095,14 +16094,14 @@
       </c>
       <c r="J108" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [588 +: 14] = deframed_mapped [1][2][10];</v>
+        <v xml:space="preserve">            parallel_daq_1 [588 +: 14] = deframed_mapped [1][2][10];</v>
       </c>
       <c r="K108" t="str">
         <f t="shared" si="10"/>
         <v>// V29</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>6</v>
       </c>
@@ -16136,14 +16135,14 @@
       </c>
       <c r="J109" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [602 +: 14] = deframed_mapped [1][2][11];</v>
+        <v xml:space="preserve">            parallel_daq_1 [602 +: 14] = deframed_mapped [1][2][11];</v>
       </c>
       <c r="K109" t="str">
         <f t="shared" si="10"/>
         <v>// U21</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>6</v>
       </c>
@@ -16177,14 +16176,14 @@
       </c>
       <c r="J110" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [616 +: 14] = deframed_mapped [1][2][12];</v>
+        <v xml:space="preserve">            parallel_daq_1 [616 +: 14] = deframed_mapped [1][2][12];</v>
       </c>
       <c r="K110" t="str">
         <f t="shared" si="10"/>
         <v>// U23</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>6</v>
       </c>
@@ -16218,14 +16217,14 @@
       </c>
       <c r="J111" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [630 +: 14] = deframed_mapped [1][2][13];</v>
+        <v xml:space="preserve">            parallel_daq_1 [630 +: 14] = deframed_mapped [1][2][13];</v>
       </c>
       <c r="K111" t="str">
         <f t="shared" si="10"/>
         <v>// U25</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>6</v>
       </c>
@@ -16259,14 +16258,14 @@
       </c>
       <c r="J112" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [644 +: 14] = deframed_mapped [1][2][14];</v>
+        <v xml:space="preserve">            parallel_daq_1 [644 +: 14] = deframed_mapped [1][2][14];</v>
       </c>
       <c r="K112" t="str">
         <f t="shared" si="10"/>
         <v>// U27</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>6</v>
       </c>
@@ -16300,14 +16299,14 @@
       </c>
       <c r="J113" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [658 +: 14] = deframed_mapped [1][2][15];</v>
+        <v xml:space="preserve">            parallel_daq_1 [658 +: 14] = deframed_mapped [1][2][15];</v>
       </c>
       <c r="K113" t="str">
         <f t="shared" si="10"/>
         <v>// U29</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>7</v>
       </c>
@@ -16341,14 +16340,14 @@
       </c>
       <c r="J114" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [672 +: 14] = deframed_mapped [1][3][0];</v>
+        <v xml:space="preserve">            parallel_daq_1 [672 +: 14] = deframed_mapped [1][3][0];</v>
       </c>
       <c r="K114" t="str">
         <f t="shared" si="10"/>
         <v>// X37</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>7</v>
       </c>
@@ -16382,14 +16381,14 @@
       </c>
       <c r="J115" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [686 +: 14] = deframed_mapped [1][3][1];</v>
+        <v xml:space="preserve">            parallel_daq_1 [686 +: 14] = deframed_mapped [1][3][1];</v>
       </c>
       <c r="K115" t="str">
         <f t="shared" si="10"/>
         <v>// X39</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>7</v>
       </c>
@@ -16423,14 +16422,14 @@
       </c>
       <c r="J116" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [700 +: 14] = deframed_mapped [1][3][2];</v>
+        <v xml:space="preserve">            parallel_daq_1 [700 +: 14] = deframed_mapped [1][3][2];</v>
       </c>
       <c r="K116" t="str">
         <f t="shared" si="10"/>
         <v>// X41</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>7</v>
       </c>
@@ -16464,14 +16463,14 @@
       </c>
       <c r="J117" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [714 +: 14] = deframed_mapped [1][3][3];</v>
+        <v xml:space="preserve">            parallel_daq_1 [714 +: 14] = deframed_mapped [1][3][3];</v>
       </c>
       <c r="K117" t="str">
         <f t="shared" si="10"/>
         <v>// X43</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>7</v>
       </c>
@@ -16505,14 +16504,14 @@
       </c>
       <c r="J118" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [728 +: 14] = deframed_mapped [1][3][4];</v>
+        <v xml:space="preserve">            parallel_daq_1 [728 +: 14] = deframed_mapped [1][3][4];</v>
       </c>
       <c r="K118" t="str">
         <f t="shared" si="10"/>
         <v>// X45</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>7</v>
       </c>
@@ -16546,14 +16545,14 @@
       </c>
       <c r="J119" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [742 +: 14] = deframed_mapped [1][3][5];</v>
+        <v xml:space="preserve">            parallel_daq_1 [742 +: 14] = deframed_mapped [1][3][5];</v>
       </c>
       <c r="K119" t="str">
         <f t="shared" si="10"/>
         <v>// X47</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>7</v>
       </c>
@@ -16587,14 +16586,14 @@
       </c>
       <c r="J120" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [756 +: 14] = deframed_mapped [1][3][6];</v>
+        <v xml:space="preserve">            parallel_daq_1 [756 +: 14] = deframed_mapped [1][3][6];</v>
       </c>
       <c r="K120" t="str">
         <f t="shared" si="10"/>
         <v>// V31</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>7</v>
       </c>
@@ -16628,14 +16627,14 @@
       </c>
       <c r="J121" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [770 +: 14] = deframed_mapped [1][3][7];</v>
+        <v xml:space="preserve">            parallel_daq_1 [770 +: 14] = deframed_mapped [1][3][7];</v>
       </c>
       <c r="K121" t="str">
         <f t="shared" si="10"/>
         <v>// V33</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>7</v>
       </c>
@@ -16669,14 +16668,14 @@
       </c>
       <c r="J122" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [784 +: 14] = deframed_mapped [1][3][8];</v>
+        <v xml:space="preserve">            parallel_daq_1 [784 +: 14] = deframed_mapped [1][3][8];</v>
       </c>
       <c r="K122" t="str">
         <f t="shared" si="10"/>
         <v>// V35</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>7</v>
       </c>
@@ -16710,14 +16709,14 @@
       </c>
       <c r="J123" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [798 +: 14] = deframed_mapped [1][3][9];</v>
+        <v xml:space="preserve">            parallel_daq_1 [798 +: 14] = deframed_mapped [1][3][9];</v>
       </c>
       <c r="K123" t="str">
         <f t="shared" si="10"/>
         <v>// V37</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>7</v>
       </c>
@@ -16751,14 +16750,14 @@
       </c>
       <c r="J124" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [812 +: 14] = deframed_mapped [1][3][10];</v>
+        <v xml:space="preserve">            parallel_daq_1 [812 +: 14] = deframed_mapped [1][3][10];</v>
       </c>
       <c r="K124" t="str">
         <f t="shared" si="10"/>
         <v>// V39</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>7</v>
       </c>
@@ -16792,14 +16791,14 @@
       </c>
       <c r="J125" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [826 +: 14] = deframed_mapped [1][3][11];</v>
+        <v xml:space="preserve">            parallel_daq_1 [826 +: 14] = deframed_mapped [1][3][11];</v>
       </c>
       <c r="K125" t="str">
         <f t="shared" si="10"/>
         <v>// U31</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>7</v>
       </c>
@@ -16833,14 +16832,14 @@
       </c>
       <c r="J126" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [840 +: 14] = deframed_mapped [1][3][12];</v>
+        <v xml:space="preserve">            parallel_daq_1 [840 +: 14] = deframed_mapped [1][3][12];</v>
       </c>
       <c r="K126" t="str">
         <f t="shared" si="10"/>
         <v>// U33</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>7</v>
       </c>
@@ -16874,14 +16873,14 @@
       </c>
       <c r="J127" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [854 +: 14] = deframed_mapped [1][3][13];</v>
+        <v xml:space="preserve">            parallel_daq_1 [854 +: 14] = deframed_mapped [1][3][13];</v>
       </c>
       <c r="K127" t="str">
         <f t="shared" si="10"/>
         <v>// U35</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>7</v>
       </c>
@@ -16915,14 +16914,14 @@
       </c>
       <c r="J128" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [868 +: 14] = deframed_mapped [1][3][14];</v>
+        <v xml:space="preserve">            parallel_daq_1 [868 +: 14] = deframed_mapped [1][3][14];</v>
       </c>
       <c r="K128" t="str">
         <f t="shared" si="10"/>
         <v>// U37</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>7</v>
       </c>
@@ -16956,7 +16955,7 @@
       </c>
       <c r="J129" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">            parallel_daq_0 [882 +: 14] = deframed_mapped [1][3][15];</v>
+        <v xml:space="preserve">            parallel_daq_1 [882 +: 14] = deframed_mapped [1][3][15];</v>
       </c>
       <c r="K129" t="str">
         <f t="shared" si="10"/>
@@ -16964,7 +16963,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D129">
+  <sortState ref="A2:D129">
     <sortCondition ref="A2:A129"/>
     <sortCondition ref="B2:B129"/>
   </sortState>

</xml_diff>